<commit_message>
experimental update - few major features have been implemented
</commit_message>
<xml_diff>
--- a/documentation/ingredients_matches.xlsx
+++ b/documentation/ingredients_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GodotProjects\Aphid Festival\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDDC723-8A45-4E35-AACD-4480FCA765D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15864328-435D-462F-8D21-4C393A08E985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>MATCHES</t>
   </si>
@@ -157,6 +157,36 @@
   </si>
   <si>
     <t>tangy_carpaccio</t>
+  </si>
+  <si>
+    <t>sweet_dew</t>
+  </si>
+  <si>
+    <t>yam_bread</t>
+  </si>
+  <si>
+    <t>frost_pie</t>
+  </si>
+  <si>
+    <t>berry_icecream</t>
+  </si>
+  <si>
+    <t>berry_jam</t>
+  </si>
+  <si>
+    <t>nutty_cake</t>
+  </si>
+  <si>
+    <t>berry_cake</t>
+  </si>
+  <si>
+    <t>honey_pancakes</t>
+  </si>
+  <si>
+    <t>berry_juice</t>
+  </si>
+  <si>
+    <t>cake</t>
   </si>
 </sst>
 </file>
@@ -497,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +639,7 @@
         <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s">
@@ -656,6 +686,7 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
+      <c r="G4" s="2"/>
       <c r="H4" t="s">
         <v>18</v>
       </c>
@@ -673,8 +704,14 @@
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="M5" s="2"/>
@@ -691,6 +728,18 @@
       <c r="F6" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
       <c r="P6" t="s">
         <v>28</v>
       </c>
@@ -708,6 +757,12 @@
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -716,7 +771,20 @@
       <c r="I9" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J9" s="2"/>
       <c r="K9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" t="s">
         <v>7</v>
       </c>
       <c r="P9" t="s">
@@ -727,7 +795,9 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">

</xml_diff>